<commit_message>
Updated: Realize the auto-login if remember-me clicked.
</commit_message>
<xml_diff>
--- a/GradutionProject/App_Data/学生选课系统数据库设计_新版.xlsx
+++ b/GradutionProject/App_Data/学生选课系统数据库设计_新版.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16160" windowHeight="8510" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="细分学科门类计划" sheetId="1" r:id="rId1"/>
@@ -174,39 +174,15 @@
     <t>datetime</t>
   </si>
   <si>
+    <t>（方案二）使用说明：每当学生选一门课程，则向该表中加入一行数据：包括学生编号、课程编号、操作类型、操作日期。</t>
+  </si>
+  <si>
     <r>
       <t>学生课程记录表（course_records）（</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>方案二</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>学生课程记录表（course_records）（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -226,17 +202,60 @@
     </r>
   </si>
   <si>
-    <t>（方案一）使用说明：学生与课程是多对多的关系，该如何使用关系型数据库建立这个数据表？目前只能使用特殊的存储结构（此处为json字符串）来进行数据的存储和取出。学生唯一编号作为login_examine表uniqueClientID字符按的外键，对于选课这个行为，它的属性有：选课行为发生的时间，选课行为的主人，所选对象（此处使用json存储所有被选的课程），课程数量（为json字符串里面的课程数量）。每当学生选一门课的时候，将jsonCid这个字段的数据取出，用json工具处理为列表，再把新选的课程id加入进去，然后再把</t>
-  </si>
-  <si>
-    <t>（方案二）使用说明：每当学生选一门课程，则向该表中加入一行数据：包括学生编号、课程编号、操作类型、操作日期。</t>
+    <r>
+      <t>学生课程记录表（course_records）（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>方案二</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>已采用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>（方案一）使用说明：学生与课程是多对多的关系，该如何使用关系型数据库建立这个数据表？目前只能使用特殊的存储结构（此处为json字符串）来进行数据的存储和取出。学生唯一编号作为login_examine表uniqueClientID字符按的外键，对于选课这个行为，它的属性有：选课行为发生的时间，选课行为的主人，所选对象（此处使用json存储所有被选的课程），课程数量（为json字符串里面的课程数量）。每当学生选一门课的时候，将jsonCid这个字段的数据取出，用json工具处理为列表，再把新选的课程id加入进去，然后再把处理过后的字符串转化为Json数据再放入数据库。（不推荐）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,8 +279,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,7 +401,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -382,7 +415,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -393,26 +435,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,11 +790,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -786,7 +822,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -803,7 +839,7 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -820,7 +856,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -837,7 +873,7 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
@@ -854,7 +890,7 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
@@ -871,7 +907,7 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
@@ -888,7 +924,7 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
@@ -905,7 +941,7 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
@@ -922,7 +958,7 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
@@ -939,7 +975,7 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
@@ -956,7 +992,7 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C13" t="s">
@@ -973,7 +1009,7 @@
       <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C14" t="s">
@@ -990,7 +1026,7 @@
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
@@ -1011,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.5" customHeight="1">
+    <row r="17" spans="1:8" ht="14.45" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1021,7 +1057,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="14.5" customHeight="1">
+    <row r="18" spans="1:8" ht="14.45" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1031,42 +1067,42 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="14.5" customHeight="1">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1083,23 +1119,23 @@
   <dimension ref="B2:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:K4"/>
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="4" width="17.08984375" customWidth="1"/>
-    <col min="7" max="7" width="4.54296875" customWidth="1"/>
-    <col min="8" max="11" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="19.453125" customWidth="1"/>
-    <col min="15" max="15" width="14.81640625" customWidth="1"/>
-    <col min="19" max="19" width="4.81640625" customWidth="1"/>
-    <col min="20" max="22" width="8.7265625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="11" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" customWidth="1"/>
+    <col min="20" max="22" width="8.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="15.5">
+    <row r="2" spans="2:22" ht="15.75">
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1109,67 +1145,67 @@
       <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="2:22">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="M3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
     </row>
     <row r="6" spans="2:22">
       <c r="B6" s="3" t="s">
@@ -1179,13 +1215,13 @@
         <v>32</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
       <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1195,13 +1231,13 @@
       <c r="O6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="7"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="10"/>
     </row>
     <row r="7" spans="2:22">
       <c r="B7" s="3" t="s">
@@ -1213,13 +1249,13 @@
       <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
       <c r="M7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1229,13 +1265,13 @@
       <c r="O7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="7"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="10"/>
     </row>
     <row r="8" spans="2:22">
       <c r="B8" s="3" t="s">
@@ -1245,15 +1281,15 @@
         <v>33</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
       <c r="M8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1263,15 +1299,15 @@
       <c r="O8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="7"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="10"/>
     </row>
     <row r="9" spans="2:22">
       <c r="B9" s="3" t="s">
@@ -1281,13 +1317,13 @@
         <v>40</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
       <c r="M9" s="3" t="s">
         <v>39</v>
       </c>
@@ -1297,13 +1333,13 @@
       <c r="O9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="10"/>
     </row>
     <row r="10" spans="2:22">
       <c r="B10" s="3" t="s">
@@ -1313,157 +1349,157 @@
         <v>42</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="7"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="10"/>
     </row>
     <row r="11" spans="2:22">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="7"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="10"/>
     </row>
     <row r="12" spans="2:22">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="7"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="10"/>
     </row>
     <row r="13" spans="2:22">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="10"/>
     </row>
     <row r="14" spans="2:22">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="7"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="10"/>
     </row>
     <row r="15" spans="2:22">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="7"/>
-    </row>
-    <row r="18" spans="2:19" ht="14.5" customHeight="1">
+      <c r="P15" s="8"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="10"/>
+    </row>
+    <row r="18" spans="2:19" ht="14.45" customHeight="1">
       <c r="B18" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="11"/>
@@ -1472,18 +1508,18 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="11"/>
@@ -1492,18 +1528,18 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="11"/>
@@ -1512,18 +1548,18 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="11"/>
@@ -1532,18 +1568,18 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="11"/>
@@ -1552,18 +1588,18 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="11"/>
@@ -1572,18 +1608,18 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="11"/>
@@ -1592,13 +1628,13 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="11"/>
@@ -1607,13 +1643,13 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="11"/>
@@ -1622,13 +1658,13 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="11"/>
@@ -1637,13 +1673,13 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="11"/>
@@ -1652,13 +1688,13 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="11"/>
@@ -1667,13 +1703,13 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="11"/>
@@ -1682,41 +1718,41 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="P15:V15"/>
+    <mergeCell ref="B18:G31"/>
+    <mergeCell ref="M18:S31"/>
+    <mergeCell ref="E15:K15"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="E13:K13"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="P10:V10"/>
+    <mergeCell ref="P11:V11"/>
+    <mergeCell ref="P12:V12"/>
+    <mergeCell ref="P13:V13"/>
+    <mergeCell ref="P14:V14"/>
     <mergeCell ref="M3:V4"/>
     <mergeCell ref="P6:V6"/>
     <mergeCell ref="P7:V7"/>
     <mergeCell ref="P8:V8"/>
     <mergeCell ref="P9:V9"/>
-    <mergeCell ref="P10:V10"/>
-    <mergeCell ref="P11:V11"/>
-    <mergeCell ref="P12:V12"/>
-    <mergeCell ref="P13:V13"/>
-    <mergeCell ref="P14:V14"/>
-    <mergeCell ref="P15:V15"/>
-    <mergeCell ref="B18:G31"/>
-    <mergeCell ref="M18:S31"/>
-    <mergeCell ref="E15:K15"/>
-    <mergeCell ref="B3:K4"/>
-    <mergeCell ref="E2:O2"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="E8:K8"/>
-    <mergeCell ref="E9:K9"/>
-    <mergeCell ref="E10:K10"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="E12:K12"/>
-    <mergeCell ref="E13:K13"/>
-    <mergeCell ref="E14:K14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1730,7 +1766,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>